<commit_message>
README and 01-data/ update
</commit_message>
<xml_diff>
--- a/01-data/241111_promoteroptimize.xlsx
+++ b/01-data/241111_promoteroptimize.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SophiaTang\Documents\normalization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SophiaTang\Documents\GitHub\benthi_variation\01-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C662847-62C7-40AA-9174-26D00DC63BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BD06CA-BBBB-4B5D-BB90-A62C5E2AF765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 1 - Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="137">
   <si>
     <t>Software Version</t>
   </si>
@@ -455,30 +455,6 @@
   </si>
   <si>
     <t>Plate 8</t>
-  </si>
-  <si>
-    <t>green CV</t>
-  </si>
-  <si>
-    <t>red CV</t>
-  </si>
-  <si>
-    <t>green/red CV</t>
-  </si>
-  <si>
-    <t>red/green CV</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>std dev</t>
-  </si>
-  <si>
-    <t>no drop</t>
-  </si>
-  <si>
-    <t>drop</t>
   </si>
 </sst>
 </file>
@@ -2170,10 +2146,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:R128"/>
+  <dimension ref="A2:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C75" workbookViewId="0">
-      <selection activeCell="O81" sqref="O81"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76:R129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2717,7 +2693,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="15" t="s">
         <v>66</v>
       </c>
@@ -2728,7 +2704,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="15" t="s">
         <v>67</v>
       </c>
@@ -2739,7 +2715,7 @@
         <v>1530</v>
       </c>
     </row>
-    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="15" t="s">
         <v>68</v>
       </c>
@@ -2750,7 +2726,7 @@
         <v>1781</v>
       </c>
     </row>
-    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="15" t="s">
         <v>69</v>
       </c>
@@ -2761,7 +2737,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="15" t="s">
         <v>70</v>
       </c>
@@ -2772,7 +2748,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="70" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="15" t="s">
         <v>71</v>
       </c>
@@ -2783,7 +2759,7 @@
         <v>1671</v>
       </c>
     </row>
-    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="15" t="s">
         <v>72</v>
       </c>
@@ -2794,7 +2770,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="15" t="s">
         <v>73</v>
       </c>
@@ -2805,7 +2781,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="15" t="s">
         <v>74</v>
       </c>
@@ -2816,7 +2792,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="74" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="15" t="s">
         <v>75</v>
       </c>
@@ -2827,7 +2803,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="15" t="s">
         <v>76</v>
       </c>
@@ -2838,7 +2814,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="76" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="15" t="s">
         <v>77</v>
       </c>
@@ -2849,7 +2825,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="15" t="s">
         <v>78</v>
       </c>
@@ -2859,20 +2835,8 @@
       <c r="D77" s="15">
         <v>1366</v>
       </c>
-      <c r="O77" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="P77" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q77" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="R77" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="78" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="15" t="s">
         <v>79</v>
       </c>
@@ -2882,46 +2846,8 @@
       <c r="D78" s="15">
         <v>1269</v>
       </c>
-      <c r="H78" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="I78" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="J78" s="8">
-        <f>AVERAGE(C81:C128)</f>
-        <v>208149.64583333334</v>
-      </c>
-      <c r="K78" s="8">
-        <f>AVERAGE(D81:D128)</f>
-        <v>2213.1875</v>
-      </c>
-      <c r="L78" s="8">
-        <f>AVERAGE(E81:E128)</f>
-        <v>94.138747979998698</v>
-      </c>
-      <c r="M78" s="8">
-        <f>AVERAGE(F81:F128)</f>
-        <v>1.2524099551353378E-2</v>
-      </c>
-      <c r="O78" s="8">
-        <f>J79/J78</f>
-        <v>0.67836679991111992</v>
-      </c>
-      <c r="P78" s="8">
-        <f>K79/K78</f>
-        <v>0.16362972092398032</v>
-      </c>
-      <c r="Q78" s="8">
-        <f>L79/L78</f>
-        <v>0.61987494756152473</v>
-      </c>
-      <c r="R78" s="8">
-        <f>M79/M78</f>
-        <v>0.27058713745870783</v>
-      </c>
-    </row>
-    <row r="79" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="15" t="s">
         <v>80</v>
       </c>
@@ -2931,27 +2857,8 @@
       <c r="D79" s="15">
         <v>1279</v>
       </c>
-      <c r="I79" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J79" s="8">
-        <f>_xlfn.STDEV.P(C81:C128)</f>
-        <v>141201.80914659132</v>
-      </c>
-      <c r="K79" s="8">
-        <f>_xlfn.STDEV.P(D81:D128)</f>
-        <v>362.1432529774417</v>
-      </c>
-      <c r="L79" s="8">
-        <f>_xlfn.STDEV.P(E81:E128)</f>
-        <v>58.354251467609288</v>
-      </c>
-      <c r="M79" s="8">
-        <f>_xlfn.STDEV.P(F81:F128)</f>
-        <v>3.3888602468485976E-3</v>
-      </c>
-    </row>
-    <row r="80" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="15" t="s">
         <v>81</v>
       </c>
@@ -2962,7 +2869,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="81" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="15" t="s">
         <v>82</v>
       </c>
@@ -2972,54 +2879,8 @@
       <c r="D81" s="15">
         <v>2878</v>
       </c>
-      <c r="E81" s="8">
-        <f>C81/D81</f>
-        <v>71.887421820708823</v>
-      </c>
-      <c r="F81" s="8">
-        <f>D81/C81</f>
-        <v>1.3910639367399415E-2</v>
-      </c>
-      <c r="H81" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="I81" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="J81" s="8">
-        <f>AVERAGE(C81:C84, C89:C128)</f>
-        <v>166700.18181818182</v>
-      </c>
-      <c r="K81" s="8">
-        <f>AVERAGE(D81:D84, D89:D128)</f>
-        <v>2196.8863636363635</v>
-      </c>
-      <c r="L81" s="8">
-        <f>AVERAGE(E81:E84, E89:E128)</f>
-        <v>77.373313023645451</v>
-      </c>
-      <c r="M81" s="8">
-        <f>AVERAGE(F81:F84, F89:F128)</f>
-        <v>1.3330370516048689E-2</v>
-      </c>
-      <c r="O81" s="8">
-        <f>J82/J81</f>
-        <v>0.14947809782272156</v>
-      </c>
-      <c r="P81" s="8">
-        <f>K82/K81</f>
-        <v>0.16951848413232043</v>
-      </c>
-      <c r="Q81" s="8">
-        <f>L82/L81</f>
-        <v>0.19250263746087212</v>
-      </c>
-      <c r="R81" s="8">
-        <f>M82/M81</f>
-        <v>0.16271228448028732</v>
-      </c>
-    </row>
-    <row r="82" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="15" t="s">
         <v>83</v>
       </c>
@@ -3029,35 +2890,8 @@
       <c r="D82" s="15">
         <v>2555</v>
       </c>
-      <c r="E82" s="8">
-        <f t="shared" ref="E82:E128" si="0">C82/D82</f>
-        <v>64.665362035225044</v>
-      </c>
-      <c r="F82" s="8">
-        <f t="shared" ref="F82:F128" si="1">D82/C82</f>
-        <v>1.5464229512165598E-2</v>
-      </c>
-      <c r="I82" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J82" s="8">
-        <f>_xlfn.STDEV.P(C81:C84,C89:C128)</f>
-        <v>24918.026084883655</v>
-      </c>
-      <c r="K82" s="8">
-        <f>_xlfn.STDEV.P(D81:D84,D89:D128)</f>
-        <v>372.41284617460201</v>
-      </c>
-      <c r="L82" s="8">
-        <f>_xlfn.STDEV.P(E81:E84,E89:E128)</f>
-        <v>14.894566826137396</v>
-      </c>
-      <c r="M82" s="8">
-        <f>_xlfn.STDEV.P(F81:F84,F89:F128)</f>
-        <v>2.1690150396349488E-3</v>
-      </c>
-    </row>
-    <row r="83" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="15" t="s">
         <v>84</v>
       </c>
@@ -3067,16 +2901,8 @@
       <c r="D83" s="15">
         <v>2184</v>
       </c>
-      <c r="E83" s="8">
-        <f t="shared" si="0"/>
-        <v>62.255494505494504</v>
-      </c>
-      <c r="F83" s="8">
-        <f t="shared" si="1"/>
-        <v>1.6062839239221569E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="15" t="s">
         <v>85</v>
       </c>
@@ -3086,16 +2912,8 @@
       <c r="D84" s="15">
         <v>2398</v>
       </c>
-      <c r="E84" s="8">
-        <f t="shared" si="0"/>
-        <v>70.116346955796502</v>
-      </c>
-      <c r="F84" s="8">
-        <f t="shared" si="1"/>
-        <v>1.4262009408881938E-2</v>
-      </c>
-    </row>
-    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="15" t="s">
         <v>86</v>
       </c>
@@ -3105,16 +2923,8 @@
       <c r="D85" s="15">
         <v>2302</v>
       </c>
-      <c r="E85" s="8">
-        <f t="shared" si="0"/>
-        <v>263.36012163336227</v>
-      </c>
-      <c r="F85" s="8">
-        <f t="shared" si="1"/>
-        <v>3.7970820859209407E-3</v>
-      </c>
-    </row>
-    <row r="86" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="15" t="s">
         <v>87</v>
       </c>
@@ -3124,16 +2934,8 @@
       <c r="D86" s="15">
         <v>2261</v>
       </c>
-      <c r="E86" s="8">
-        <f t="shared" si="0"/>
-        <v>319.25563909774434</v>
-      </c>
-      <c r="F86" s="8">
-        <f t="shared" si="1"/>
-        <v>3.1322860978309506E-3</v>
-      </c>
-    </row>
-    <row r="87" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="15" t="s">
         <v>88</v>
       </c>
@@ -3143,16 +2945,8 @@
       <c r="D87" s="15">
         <v>2470</v>
       </c>
-      <c r="E87" s="8">
-        <f t="shared" si="0"/>
-        <v>304.96720647773282</v>
-      </c>
-      <c r="F87" s="8">
-        <f t="shared" si="1"/>
-        <v>3.2790410862520562E-3</v>
-      </c>
-    </row>
-    <row r="88" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="15" t="s">
         <v>89</v>
       </c>
@@ -3162,16 +2956,8 @@
       <c r="D88" s="15">
         <v>2537</v>
       </c>
-      <c r="E88" s="8">
-        <f t="shared" si="0"/>
-        <v>226.65116279069767</v>
-      </c>
-      <c r="F88" s="8">
-        <f t="shared" si="1"/>
-        <v>4.4120664888159244E-3</v>
-      </c>
-    </row>
-    <row r="89" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="15" t="s">
         <v>90</v>
       </c>
@@ -3181,16 +2967,8 @@
       <c r="D89" s="15">
         <v>2862</v>
       </c>
-      <c r="E89" s="8">
-        <f t="shared" si="0"/>
-        <v>59.758909853249477</v>
-      </c>
-      <c r="F89" s="8">
-        <f t="shared" si="1"/>
-        <v>1.6733906332222416E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="15" t="s">
         <v>91</v>
       </c>
@@ -3200,16 +2978,8 @@
       <c r="D90" s="15">
         <v>2742</v>
       </c>
-      <c r="E90" s="8">
-        <f t="shared" si="0"/>
-        <v>68.070021881838073</v>
-      </c>
-      <c r="F90" s="8">
-        <f t="shared" si="1"/>
-        <v>1.4690754789764691E-2</v>
-      </c>
-    </row>
-    <row r="91" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="15" t="s">
         <v>92</v>
       </c>
@@ -3219,16 +2989,8 @@
       <c r="D91" s="15">
         <v>3113</v>
       </c>
-      <c r="E91" s="8">
-        <f t="shared" si="0"/>
-        <v>66.118213941535501</v>
-      </c>
-      <c r="F91" s="8">
-        <f t="shared" si="1"/>
-        <v>1.5124425485604345E-2</v>
-      </c>
-    </row>
-    <row r="92" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="15" t="s">
         <v>93</v>
       </c>
@@ -3238,16 +3000,8 @@
       <c r="D92" s="15">
         <v>2665</v>
       </c>
-      <c r="E92" s="8">
-        <f t="shared" si="0"/>
-        <v>85.121575984990614</v>
-      </c>
-      <c r="F92" s="8">
-        <f t="shared" si="1"/>
-        <v>1.1747902789961604E-2</v>
-      </c>
-    </row>
-    <row r="93" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="15" t="s">
         <v>94</v>
       </c>
@@ -3257,16 +3011,8 @@
       <c r="D93" s="15">
         <v>2254</v>
       </c>
-      <c r="E93" s="8">
-        <f t="shared" si="0"/>
-        <v>67.975598935226259</v>
-      </c>
-      <c r="F93" s="8">
-        <f t="shared" si="1"/>
-        <v>1.4711161294112271E-2</v>
-      </c>
-    </row>
-    <row r="94" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" s="15" t="s">
         <v>95</v>
       </c>
@@ -3276,16 +3022,8 @@
       <c r="D94" s="15">
         <v>1771</v>
       </c>
-      <c r="E94" s="8">
-        <f t="shared" si="0"/>
-        <v>71.735177865612641</v>
-      </c>
-      <c r="F94" s="8">
-        <f t="shared" si="1"/>
-        <v>1.3940161992396276E-2</v>
-      </c>
-    </row>
-    <row r="95" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="15" t="s">
         <v>96</v>
       </c>
@@ -3295,16 +3033,8 @@
       <c r="D95" s="15">
         <v>2465</v>
       </c>
-      <c r="E95" s="8">
-        <f t="shared" si="0"/>
-        <v>67.576064908722103</v>
-      </c>
-      <c r="F95" s="8">
-        <f t="shared" si="1"/>
-        <v>1.4798138976437041E-2</v>
-      </c>
-    </row>
-    <row r="96" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" s="15" t="s">
         <v>97</v>
       </c>
@@ -3314,16 +3044,8 @@
       <c r="D96" s="15">
         <v>1519</v>
       </c>
-      <c r="E96" s="8">
-        <f t="shared" si="0"/>
-        <v>128.32126398946676</v>
-      </c>
-      <c r="F96" s="8">
-        <f t="shared" si="1"/>
-        <v>7.7929406936178948E-3</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="15" t="s">
         <v>98</v>
       </c>
@@ -3333,16 +3055,8 @@
       <c r="D97" s="15">
         <v>2366</v>
       </c>
-      <c r="E97" s="8">
-        <f t="shared" si="0"/>
-        <v>69.550718512256978</v>
-      </c>
-      <c r="F97" s="8">
-        <f t="shared" si="1"/>
-        <v>1.4377996682000765E-2</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="15" t="s">
         <v>99</v>
       </c>
@@ -3352,16 +3066,8 @@
       <c r="D98" s="15">
         <v>2863</v>
       </c>
-      <c r="E98" s="8">
-        <f t="shared" si="0"/>
-        <v>60.263709395738736</v>
-      </c>
-      <c r="F98" s="8">
-        <f t="shared" si="1"/>
-        <v>1.6593734604572984E-2</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="15" t="s">
         <v>100</v>
       </c>
@@ -3371,16 +3077,8 @@
       <c r="D99" s="15">
         <v>2090</v>
       </c>
-      <c r="E99" s="8">
-        <f t="shared" si="0"/>
-        <v>65.390430622009575</v>
-      </c>
-      <c r="F99" s="8">
-        <f t="shared" si="1"/>
-        <v>1.5292757525646466E-2</v>
-      </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="15" t="s">
         <v>101</v>
       </c>
@@ -3390,16 +3088,8 @@
       <c r="D100" s="15">
         <v>2877</v>
       </c>
-      <c r="E100" s="8">
-        <f t="shared" si="0"/>
-        <v>60.202641640597847</v>
-      </c>
-      <c r="F100" s="8">
-        <f t="shared" si="1"/>
-        <v>1.6610566791568276E-2</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="15" t="s">
         <v>102</v>
       </c>
@@ -3409,16 +3099,8 @@
       <c r="D101" s="15">
         <v>1654</v>
       </c>
-      <c r="E101" s="8">
-        <f t="shared" si="0"/>
-        <v>110.80290205562274</v>
-      </c>
-      <c r="F101" s="8">
-        <f t="shared" si="1"/>
-        <v>9.0250343758866789E-3</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="15" t="s">
         <v>103</v>
       </c>
@@ -3428,16 +3110,8 @@
       <c r="D102" s="15">
         <v>2080</v>
       </c>
-      <c r="E102" s="8">
-        <f t="shared" si="0"/>
-        <v>77.264903846153842</v>
-      </c>
-      <c r="F102" s="8">
-        <f t="shared" si="1"/>
-        <v>1.2942486824175072E-2</v>
-      </c>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="15" t="s">
         <v>104</v>
       </c>
@@ -3447,16 +3121,8 @@
       <c r="D103" s="15">
         <v>2256</v>
       </c>
-      <c r="E103" s="8">
-        <f t="shared" si="0"/>
-        <v>99.776152482269509</v>
-      </c>
-      <c r="F103" s="8">
-        <f t="shared" si="1"/>
-        <v>1.0022434971900753E-2</v>
-      </c>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="15" t="s">
         <v>105</v>
       </c>
@@ -3466,16 +3132,8 @@
       <c r="D104" s="15">
         <v>2031</v>
       </c>
-      <c r="E104" s="8">
-        <f t="shared" si="0"/>
-        <v>78.50320039389463</v>
-      </c>
-      <c r="F104" s="8">
-        <f t="shared" si="1"/>
-        <v>1.2738334169593577E-2</v>
-      </c>
-    </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="15" t="s">
         <v>106</v>
       </c>
@@ -3485,16 +3143,8 @@
       <c r="D105" s="15">
         <v>2294</v>
       </c>
-      <c r="E105" s="8">
-        <f t="shared" si="0"/>
-        <v>84.001307759372281</v>
-      </c>
-      <c r="F105" s="8">
-        <f t="shared" si="1"/>
-        <v>1.1904576567600246E-2</v>
-      </c>
-    </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="15" t="s">
         <v>107</v>
       </c>
@@ -3504,16 +3154,8 @@
       <c r="D106" s="15">
         <v>2075</v>
       </c>
-      <c r="E106" s="8">
-        <f t="shared" si="0"/>
-        <v>73.341686746987946</v>
-      </c>
-      <c r="F106" s="8">
-        <f t="shared" si="1"/>
-        <v>1.3634810492561636E-2</v>
-      </c>
-    </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" s="15" t="s">
         <v>108</v>
       </c>
@@ -3523,16 +3165,8 @@
       <c r="D107" s="15">
         <v>2047</v>
       </c>
-      <c r="E107" s="8">
-        <f t="shared" si="0"/>
-        <v>84.729360039081584</v>
-      </c>
-      <c r="F107" s="8">
-        <f t="shared" si="1"/>
-        <v>1.1802284350297796E-2</v>
-      </c>
-    </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" s="15" t="s">
         <v>109</v>
       </c>
@@ -3542,16 +3176,8 @@
       <c r="D108" s="15">
         <v>2135</v>
       </c>
-      <c r="E108" s="8">
-        <f t="shared" si="0"/>
-        <v>66.868384074941446</v>
-      </c>
-      <c r="F108" s="8">
-        <f t="shared" si="1"/>
-        <v>1.4954750497324256E-2</v>
-      </c>
-    </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="15" t="s">
         <v>110</v>
       </c>
@@ -3561,16 +3187,8 @@
       <c r="D109" s="15">
         <v>1963</v>
       </c>
-      <c r="E109" s="8">
-        <f t="shared" si="0"/>
-        <v>75.284258787570039</v>
-      </c>
-      <c r="F109" s="8">
-        <f t="shared" si="1"/>
-        <v>1.3282989247748388E-2</v>
-      </c>
-    </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="15" t="s">
         <v>111</v>
       </c>
@@ -3580,16 +3198,8 @@
       <c r="D110" s="15">
         <v>1941</v>
       </c>
-      <c r="E110" s="8">
-        <f t="shared" si="0"/>
-        <v>80.766099948480161</v>
-      </c>
-      <c r="F110" s="8">
-        <f t="shared" si="1"/>
-        <v>1.2381432316750337E-2</v>
-      </c>
-    </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="15" t="s">
         <v>112</v>
       </c>
@@ -3599,16 +3209,8 @@
       <c r="D111" s="15">
         <v>2140</v>
       </c>
-      <c r="E111" s="8">
-        <f t="shared" si="0"/>
-        <v>89.013084112149528</v>
-      </c>
-      <c r="F111" s="8">
-        <f t="shared" si="1"/>
-        <v>1.1234303473184663E-2</v>
-      </c>
-    </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="15" t="s">
         <v>113</v>
       </c>
@@ -3618,16 +3220,8 @@
       <c r="D112" s="15">
         <v>1807</v>
       </c>
-      <c r="E112" s="8">
-        <f t="shared" si="0"/>
-        <v>87.263973436635311</v>
-      </c>
-      <c r="F112" s="8">
-        <f t="shared" si="1"/>
-        <v>1.1459482769554684E-2</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="15" t="s">
         <v>114</v>
       </c>
@@ -3637,16 +3231,8 @@
       <c r="D113" s="15">
         <v>2225</v>
       </c>
-      <c r="E113" s="8">
-        <f t="shared" si="0"/>
-        <v>65.736629213483141</v>
-      </c>
-      <c r="F113" s="8">
-        <f t="shared" si="1"/>
-        <v>1.5212219001258E-2</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="15" t="s">
         <v>115</v>
       </c>
@@ -3656,16 +3242,8 @@
       <c r="D114" s="15">
         <v>2055</v>
       </c>
-      <c r="E114" s="8">
-        <f t="shared" si="0"/>
-        <v>67.861800486618009</v>
-      </c>
-      <c r="F114" s="8">
-        <f t="shared" si="1"/>
-        <v>1.4735830656264342E-2</v>
-      </c>
-    </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="15" t="s">
         <v>116</v>
       </c>
@@ -3675,16 +3253,8 @@
       <c r="D115" s="15">
         <v>2665</v>
       </c>
-      <c r="E115" s="8">
-        <f t="shared" si="0"/>
-        <v>63.853283302063787</v>
-      </c>
-      <c r="F115" s="8">
-        <f t="shared" si="1"/>
-        <v>1.5660901809377736E-2</v>
-      </c>
-    </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="15" t="s">
         <v>117</v>
       </c>
@@ -3694,16 +3264,8 @@
       <c r="D116" s="15">
         <v>1910</v>
       </c>
-      <c r="E116" s="8">
-        <f t="shared" si="0"/>
-        <v>79.534554973821983</v>
-      </c>
-      <c r="F116" s="8">
-        <f t="shared" si="1"/>
-        <v>1.2573151384692352E-2</v>
-      </c>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="15" t="s">
         <v>118</v>
       </c>
@@ -3713,16 +3275,8 @@
       <c r="D117" s="15">
         <v>2088</v>
       </c>
-      <c r="E117" s="8">
-        <f t="shared" si="0"/>
-        <v>59.655172413793103</v>
-      </c>
-      <c r="F117" s="8">
-        <f t="shared" si="1"/>
-        <v>1.6763005780346819E-2</v>
-      </c>
-    </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="15" t="s">
         <v>119</v>
       </c>
@@ -3732,16 +3286,8 @@
       <c r="D118" s="15">
         <v>1802</v>
       </c>
-      <c r="E118" s="8">
-        <f t="shared" si="0"/>
-        <v>90.359045504994455</v>
-      </c>
-      <c r="F118" s="8">
-        <f t="shared" si="1"/>
-        <v>1.1066960639206029E-2</v>
-      </c>
-    </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="15" t="s">
         <v>120</v>
       </c>
@@ -3751,16 +3297,8 @@
       <c r="D119" s="15">
         <v>2041</v>
       </c>
-      <c r="E119" s="8">
-        <f t="shared" si="0"/>
-        <v>84.263106320431163</v>
-      </c>
-      <c r="F119" s="8">
-        <f t="shared" si="1"/>
-        <v>1.1867590024479449E-2</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" s="15" t="s">
         <v>121</v>
       </c>
@@ -3770,16 +3308,8 @@
       <c r="D120" s="15">
         <v>1682</v>
       </c>
-      <c r="E120" s="8">
-        <f t="shared" si="0"/>
-        <v>75.897740784780027</v>
-      </c>
-      <c r="F120" s="8">
-        <f t="shared" si="1"/>
-        <v>1.3175622747924174E-2</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="15" t="s">
         <v>122</v>
       </c>
@@ -3789,16 +3319,8 @@
       <c r="D121" s="15">
         <v>2197</v>
       </c>
-      <c r="E121" s="8">
-        <f t="shared" si="0"/>
-        <v>70.131998179335454</v>
-      </c>
-      <c r="F121" s="8">
-        <f t="shared" si="1"/>
-        <v>1.4258826583592938E-2</v>
-      </c>
-    </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" s="15" t="s">
         <v>123</v>
       </c>
@@ -3808,16 +3330,8 @@
       <c r="D122" s="15">
         <v>2290</v>
       </c>
-      <c r="E122" s="8">
-        <f t="shared" si="0"/>
-        <v>77.893449781659385</v>
-      </c>
-      <c r="F122" s="8">
-        <f t="shared" si="1"/>
-        <v>1.2838049961878279E-2</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="15" t="s">
         <v>124</v>
       </c>
@@ -3827,16 +3341,8 @@
       <c r="D123" s="15">
         <v>1914</v>
       </c>
-      <c r="E123" s="8">
-        <f t="shared" si="0"/>
-        <v>116.90961337513062</v>
-      </c>
-      <c r="F123" s="8">
-        <f t="shared" si="1"/>
-        <v>8.5536165173284474E-3</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="15" t="s">
         <v>125</v>
       </c>
@@ -3846,16 +3352,8 @@
       <c r="D124" s="15">
         <v>2172</v>
       </c>
-      <c r="E124" s="8">
-        <f t="shared" si="0"/>
-        <v>68.280847145488025</v>
-      </c>
-      <c r="F124" s="8">
-        <f t="shared" si="1"/>
-        <v>1.4645395331274527E-2</v>
-      </c>
-    </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="15" t="s">
         <v>126</v>
       </c>
@@ -3865,16 +3363,8 @@
       <c r="D125" s="15">
         <v>1702</v>
       </c>
-      <c r="E125" s="8">
-        <f t="shared" si="0"/>
-        <v>83.472385428907174</v>
-      </c>
-      <c r="F125" s="8">
-        <f t="shared" si="1"/>
-        <v>1.1980009854297178E-2</v>
-      </c>
-    </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="15" t="s">
         <v>127</v>
       </c>
@@ -3884,16 +3374,8 @@
       <c r="D126" s="15">
         <v>1942</v>
       </c>
-      <c r="E126" s="8">
-        <f t="shared" si="0"/>
-        <v>82.769309989701341</v>
-      </c>
-      <c r="F126" s="8">
-        <f t="shared" si="1"/>
-        <v>1.2081772822854582E-2</v>
-      </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" s="15" t="s">
         <v>128</v>
       </c>
@@ -3903,16 +3385,8 @@
       <c r="D127" s="15">
         <v>2161</v>
       </c>
-      <c r="E127" s="8">
-        <f t="shared" si="0"/>
-        <v>76.622859787135582</v>
-      </c>
-      <c r="F127" s="8">
-        <f t="shared" si="1"/>
-        <v>1.3050935488156926E-2</v>
-      </c>
-    </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" s="15" t="s">
         <v>129</v>
       </c>
@@ -3921,14 +3395,6 @@
       </c>
       <c r="D128" s="15">
         <v>1792</v>
-      </c>
-      <c r="E128" s="8">
-        <f t="shared" si="0"/>
-        <v>94.559709821428569</v>
-      </c>
-      <c r="F128" s="8">
-        <f t="shared" si="1"/>
-        <v>1.0575328561058949E-2</v>
       </c>
     </row>
   </sheetData>
@@ -5200,7 +4666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:D128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>

</xml_diff>